<commit_message>
successful test at Prison Bowl 2022
</commit_message>
<xml_diff>
--- a/inputs/master_templates/29_playoffs.xlsx
+++ b/inputs/master_templates/29_playoffs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorprieto/Desktop/code/cornerstone/inputs/master_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004ercu\Desktop\python\cornerstone\master templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7884C-1CBF-9A4D-B1B4-140035B912C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0F86CB-96AA-4082-92FD-718755D5745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="tournament format" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="141">
   <si>
     <t>Team</t>
   </si>
@@ -212,9 +214,6 @@
     <t>Team E5</t>
   </si>
   <si>
-    <t>Team E6</t>
-  </si>
-  <si>
     <t>Room 13</t>
   </si>
   <si>
@@ -458,9 +457,6 @@
     <t>TE5</t>
   </si>
   <si>
-    <t>TE6</t>
-  </si>
-  <si>
     <t>Championship A</t>
   </si>
   <si>
@@ -485,10 +481,10 @@
     <t>6,6,6,6,5</t>
   </si>
   <si>
-    <t>1,11,3,9,5,7,12,2,10,4,8,6,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29</t>
-  </si>
-  <si>
     <t>crossover</t>
+  </si>
+  <si>
+    <t>1,12,4,9,5,8,2,11,3,10,6,7,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29</t>
   </si>
 </sst>
 </file>
@@ -582,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -696,13 +692,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -772,6 +779,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1092,11 +1102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE5B6E-5562-4B4B-9B01-3722A29F012F}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="42.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
@@ -1105,123 +1113,123 @@
   <sheetData>
     <row r="1" spans="1:3" ht="40" customHeight="1">
       <c r="A1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>68</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="40" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="40" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="40" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="40" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="40" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="40" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="40" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="40" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="40" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>140</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="40" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1232,14 +1240,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0CB595-5535-8C4C-9710-F68F5657C36B}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="28.109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="7.77734375" style="3" customWidth="1"/>
@@ -1253,16 +1261,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1270,7 +1278,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" s="16" t="str">
         <f>'group names'!A$2</f>
@@ -1280,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1288,7 +1296,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="14" t="str">
         <f>'group names'!A$2</f>
@@ -1298,7 +1306,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1306,7 +1314,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="11" t="str">
         <f>'group names'!A$2</f>
@@ -1316,7 +1324,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1324,7 +1332,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="11" t="str">
         <f>'group names'!A$2</f>
@@ -1334,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1342,7 +1350,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="11" t="str">
         <f>'group names'!A$2</f>
@@ -1352,7 +1360,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1360,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="11" t="str">
         <f>'group names'!A$2</f>
@@ -1370,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1378,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="11" t="str">
         <f>'group names'!A$3</f>
@@ -1388,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1396,7 +1404,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="11" t="str">
         <f>'group names'!A$3</f>
@@ -1406,7 +1414,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1414,7 +1422,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="11" t="str">
         <f>'group names'!A$3</f>
@@ -1424,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1432,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C11" s="11" t="str">
         <f>'group names'!A$3</f>
@@ -1442,7 +1450,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1450,7 +1458,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="11" t="str">
         <f>'group names'!A$3</f>
@@ -1460,7 +1468,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1468,7 +1476,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="11" t="str">
         <f>'group names'!A$3</f>
@@ -1478,7 +1486,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1486,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="11" t="str">
         <f>'group names'!A$4</f>
@@ -1496,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1504,7 +1512,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="11" t="str">
         <f>'group names'!A$4</f>
@@ -1514,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1522,7 +1530,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="11" t="str">
         <f>'group names'!A$4</f>
@@ -1532,7 +1540,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1540,7 +1548,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" s="11" t="str">
         <f>'group names'!A$4</f>
@@ -1550,7 +1558,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1558,7 +1566,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" s="11" t="str">
         <f>'group names'!A$4</f>
@@ -1568,7 +1576,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1576,7 +1584,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="11" t="str">
         <f>'group names'!A$4</f>
@@ -1586,7 +1594,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1594,7 +1602,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" s="11" t="str">
         <f>'group names'!A$5</f>
@@ -1604,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1612,7 +1620,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" s="11" t="str">
         <f>'group names'!A$5</f>
@@ -1622,7 +1630,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1630,7 +1638,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="11" t="str">
         <f>'group names'!A$5</f>
@@ -1640,7 +1648,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1648,7 +1656,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="11" t="str">
         <f>'group names'!A$5</f>
@@ -1658,7 +1666,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1666,7 +1674,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="11" t="str">
         <f>'group names'!A$5</f>
@@ -1676,7 +1684,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1684,7 +1692,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" s="11" t="str">
         <f>'group names'!A$5</f>
@@ -1694,7 +1702,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1702,7 +1710,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26" s="11" t="str">
         <f>'group names'!A$6</f>
@@ -1712,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1720,7 +1728,7 @@
         <v>45</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="11" t="str">
         <f>'group names'!A$6</f>
@@ -1730,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1738,7 +1746,7 @@
         <v>47</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C28" s="11" t="str">
         <f>'group names'!A$6</f>
@@ -1748,7 +1756,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1756,7 +1764,7 @@
         <v>48</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C29" s="11" t="str">
         <f>'group names'!A$6</f>
@@ -1766,7 +1774,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1774,7 +1782,7 @@
         <v>49</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" s="11" t="str">
         <f>'group names'!A$6</f>
@@ -1784,25 +1792,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="11" t="str">
-        <f>'group names'!A$6</f>
-        <v>Group E</v>
-      </c>
-      <c r="D31" s="18">
-        <v>6</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1818,7 +1808,7 @@
   <sheetViews>
     <sheetView zoomScale="244" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="25.21875" customWidth="1"/>
     <col min="2" max="2" width="28.44140625" customWidth="1"/>
@@ -1826,10 +1816,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="36" customHeight="1">
       <c r="A1" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="36" customHeight="1">
@@ -1837,7 +1827,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="36" customHeight="1">
@@ -1845,7 +1835,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="36" customHeight="1">
@@ -1853,7 +1843,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="36" customHeight="1">
@@ -1861,7 +1851,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="36" customHeight="1">
@@ -1869,7 +1859,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1907,7 +1897,7 @@
   <sheetViews>
     <sheetView zoomScale="184" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" customWidth="1"/>
@@ -1919,7 +1909,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>43</v>
@@ -2071,7 +2061,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="4" t="str">
         <f>'group names'!B$6</f>
@@ -2083,7 +2073,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>'group names'!B$6</f>
@@ -2095,7 +2085,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>'group names'!B$6</f>
@@ -2118,7 +2108,7 @@
   <sheetViews>
     <sheetView zoomScale="184" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="26.21875" customWidth="1"/>
@@ -2128,100 +2118,100 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2238,7 +2228,7 @@
   <sheetViews>
     <sheetView zoomScale="184" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
     <col min="2" max="2" width="47.109375" customWidth="1"/>
@@ -2246,26 +2236,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="40" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="160" customHeight="1">
       <c r="A2" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="160" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>